<commit_message>
Evosys Fusion Scenarios Added: Split,Merge,Approval of Invoice
</commit_message>
<xml_diff>
--- a/automation-project/ExcelDataFiles/ConfigurationDetails.xlsx
+++ b/automation-project/ExcelDataFiles/ConfigurationDetails.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>URL Details</t>
   </si>
@@ -63,24 +63,12 @@
     <t>Automation DB Password</t>
   </si>
   <si>
-    <t>D:\\Docs\\Rahul\\VitaminShopee\\Automation_Project\\exe\\IEDriverServer.exe</t>
-  </si>
-  <si>
-    <t>D:\\Docs\\Rahul\\VitaminShopee\\Automation_Project\\exe\\chromedriver.exe</t>
-  </si>
-  <si>
-    <t>D:\\Docs\\Rahul\\VitaminShopee\\Automation_Project\\exe\\geckodriver.exe</t>
-  </si>
-  <si>
     <t>https://www.amazon.in/</t>
   </si>
   <si>
     <t>https://www.amazon.com/</t>
   </si>
   <si>
-    <t>jdbc:mysql://127.0.0.1:3306/vitaminshopeeautomationdb</t>
-  </si>
-  <si>
     <t>Mobile Environment</t>
   </si>
   <si>
@@ -142,6 +130,30 @@
   </si>
   <si>
     <t>https://www.specsavers.co.uk/frame-styler</t>
+  </si>
+  <si>
+    <t>jdbc:mysql://127.0.0.1:3306/automationdb</t>
+  </si>
+  <si>
+    <t>C:\\Users\\vaibhav13011\\git\\staf\\Automatix-FPT\\automation-project\\exe\\IEDriverServer.exe</t>
+  </si>
+  <si>
+    <t>C:\\Users\\vaibhav13011\\git\\staf\\Automatix-FPT\\automation-project\\exe\\chromedriver.exe</t>
+  </si>
+  <si>
+    <t>C:\\Users\\vaibhav13011\\git\\staf\\Automatix-FPT\\automation-project\\exe\\geckodriver.exe</t>
+  </si>
+  <si>
+    <t>Ranorex Test Env</t>
+  </si>
+  <si>
+    <t>https://www.ranorex.com/web-testing-examples/vip/</t>
+  </si>
+  <si>
+    <t>Evosys Test Env</t>
+  </si>
+  <si>
+    <t>https://eibf-test.login.em2.oraclecloud.com/</t>
   </si>
 </sst>
 </file>
@@ -570,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:XFD41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +597,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -594,178 +606,196 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -773,9 +803,11 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added system path for chromedriver
</commit_message>
<xml_diff>
--- a/automation-project/ExcelDataFiles/ConfigurationDetails.xlsx
+++ b/automation-project/ExcelDataFiles/ConfigurationDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>C:\\Users\\vaibhav13011\\git\\staf\\Automatix-FPT\\automation-project\\exe\\IEDriverServer.exe</t>
   </si>
   <si>
-    <t>C:\\Users\\vaibhav13011\\git\\staf\\Automatix-FPT\\automation-project\\exe\\chromedriver.exe</t>
-  </si>
-  <si>
     <t>C:\\Users\\vaibhav13011\\git\\staf\\Automatix-FPT\\automation-project\\exe\\geckodriver.exe</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>https://eibf-test.login.em2.oraclecloud.com/</t>
+  </si>
+  <si>
+    <t>\\exe\\chromedriver.exe</t>
   </si>
 </sst>
 </file>
@@ -585,17 +585,17 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="51.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="49.44140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="51.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="52.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="51.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -613,7 +613,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -622,7 +622,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -631,7 +631,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -640,25 +640,25 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -669,7 +669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -680,7 +680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -707,7 +707,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -716,7 +716,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -725,7 +725,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -734,7 +734,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -743,25 +743,25 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>39</v>
+      <c r="B17" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -770,7 +770,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -779,7 +779,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -788,7 +788,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -805,9 +805,10 @@
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B17" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -817,7 +818,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -829,7 +830,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>